<commit_message>
Fixes make-ids & partial data loss in convert to/from indent
- Left pad IDs with 0s to 7 digits
- read only data from xlsx (not fromulas)
</commit_message>
<xml_diff>
--- a/tests/data/concept-scheme-simple.xlsx
+++ b/tests/data/concept-scheme-simple.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\TA1\github\voc4cat-tool\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\nfdi4cat\gh-dalito\voc4cat-tool\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD71C94-0C4B-4C42-AAE2-2F341584998C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4DA7B9-6B8F-494D-9F9A-CF094D4D816D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1065" windowWidth="24915" windowHeight="16335" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -356,9 +356,6 @@
     <t>0.1</t>
   </si>
   <si>
-    <t>ex:test</t>
-  </si>
-  <si>
     <t>en</t>
   </si>
   <si>
@@ -504,6 +501,9 @@
   </si>
   <si>
     <t>con</t>
+  </si>
+  <si>
+    <t>ex:test/</t>
   </si>
 </sst>
 </file>
@@ -757,14 +757,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -775,12 +781,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1134,7 +1134,7 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="32" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="33"/>
@@ -1201,7 +1201,7 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="32" t="s">
         <v>1</v>
       </c>
       <c r="I7" s="33"/>
@@ -1216,7 +1216,7 @@
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
-      <c r="H8" s="40" t="s">
+      <c r="H8" s="35" t="s">
         <v>2</v>
       </c>
       <c r="I8" s="33"/>
@@ -1231,7 +1231,7 @@
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="35"/>
+      <c r="H9" s="36"/>
       <c r="I9" s="33"/>
       <c r="J9" s="33"/>
       <c r="K9" s="19"/>
@@ -1244,7 +1244,7 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="35" t="s">
+      <c r="H10" s="36" t="s">
         <v>3</v>
       </c>
       <c r="I10" s="33"/>
@@ -1289,7 +1289,7 @@
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
-      <c r="H13" s="36" t="s">
+      <c r="H13" s="38" t="s">
         <v>6</v>
       </c>
       <c r="I13" s="33"/>
@@ -1304,7 +1304,7 @@
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="35" t="s">
+      <c r="H14" s="36" t="s">
         <v>7</v>
       </c>
       <c r="I14" s="33"/>
@@ -1325,11 +1325,11 @@
       <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="33"/>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="40" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="33"/>
@@ -1342,11 +1342,11 @@
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="39" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="33"/>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="34" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="33"/>
@@ -1372,7 +1372,7 @@
       <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="37" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="33"/>
@@ -1426,7 +1426,7 @@
       <c r="K22" s="19"/>
     </row>
     <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="36" t="s">
         <v>13</v>
       </c>
       <c r="B23" s="33"/>
@@ -1454,7 +1454,7 @@
       <c r="K24" s="19"/>
     </row>
     <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="37" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="33"/>
@@ -1482,7 +1482,7 @@
       <c r="K26" s="19"/>
     </row>
     <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="37" t="s">
         <v>15</v>
       </c>
       <c r="B27" s="33"/>
@@ -2488,11 +2488,6 @@
     <row r="1005" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="A25:G25"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="H10:J10"/>
@@ -2503,6 +2498,11 @@
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="A25:G25"/>
   </mergeCells>
   <conditionalFormatting sqref="H17:J18 K1:K8 K17:K28 H3:J7 H10:J10 H8 K10:K15 H13:J13 H14 A18:G18 A15:J15 A19:J28 A10:G14 A2:G8 A1:J1 A9:K9">
     <cfRule type="containsBlanks" dxfId="8" priority="13">
@@ -2561,7 +2561,7 @@
   <dimension ref="A1:D999"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2585,7 +2585,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -2599,7 +2599,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>21</v>
@@ -2613,7 +2613,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>24</v>
@@ -2697,7 +2697,7 @@
         <v>39</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>40</v>
@@ -5710,8 +5710,8 @@
   </sheetPr>
   <dimension ref="A1:I523"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5760,179 +5760,179 @@
         <v>53</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" s="27" t="s">
+      <c r="I3" s="27" t="s">
         <v>87</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G4" s="24"/>
       <c r="H4" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="27" t="s">
         <v>90</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="H5" s="27" t="s">
+      <c r="I5" s="27" t="s">
         <v>93</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G6" s="28"/>
       <c r="H6" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="27" t="s">
         <v>95</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="27" t="s">
+      <c r="E7" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="27" t="s">
         <v>108</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>109</v>
       </c>
       <c r="G7" s="28"/>
       <c r="H7" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7" s="27" t="s">
         <v>110</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="27" t="s">
+      <c r="E8" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="27" t="s">
         <v>113</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>114</v>
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="I8" s="27" t="s">
         <v>115</v>
-      </c>
-      <c r="I8" s="27" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6534,19 +6534,19 @@
         <v>ex:test/term1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>105</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6647,7 +6647,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -6688,19 +6688,19 @@
     </row>
     <row r="3" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>117</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add ci-check to wrapper.main
Update data files for testing to conform to checks.
Add tests for ci-check and use new config update method.
</commit_message>
<xml_diff>
--- a/tests/data/concept-scheme-simple.xlsx
+++ b/tests/data/concept-scheme-simple.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\nfdi4cat\gh-dalito\voc4cat-tool\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-tool\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4DA7B9-6B8F-494D-9F9A-CF094D4D816D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C71C26-CD73-41A5-B4F0-10140999E549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25095" windowHeight="15825" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="115">
   <si>
     <t xml:space="preserve">Created by </t>
   </si>
@@ -146,9 +146,6 @@
     <t>Surround Australia Pty Ltd</t>
   </si>
   <si>
-    <t xml:space="preserve">and distributed under  GPL-3.0 License </t>
-  </si>
-  <si>
     <t>SKOS Vocabulary Template</t>
   </si>
   <si>
@@ -266,9 +263,6 @@
     <t>Custodian</t>
   </si>
   <si>
-    <t>David Linke</t>
-  </si>
-  <si>
     <t>Vocabulary Content Manager</t>
   </si>
   <si>
@@ -377,57 +371,21 @@
     <t>term4</t>
   </si>
   <si>
-    <t>ex:test/term2, ex:test/term3</t>
-  </si>
-  <si>
-    <t>ex:test/term4</t>
-  </si>
-  <si>
-    <t>ex:test/term1,
-ex:test/term2,
-ex:test/term3,
-ex:test/term4</t>
-  </si>
-  <si>
     <t>voc4cat-test-data</t>
   </si>
   <si>
     <t>A concept scheme for unit testing voc4cat.</t>
   </si>
   <si>
-    <t>Leibniz-Institut für Katalyse e.V. (LIKAT)</t>
-  </si>
-  <si>
-    <t>ex:test/term1</t>
-  </si>
-  <si>
-    <t>Prov for term1</t>
-  </si>
-  <si>
     <t>ex:XYZ/term1</t>
   </si>
   <si>
-    <t>ex:test/term2</t>
-  </si>
-  <si>
-    <t>Prov for term2</t>
-  </si>
-  <si>
     <t>ex:XYZ/term2</t>
   </si>
   <si>
-    <t>ex:test/term3</t>
-  </si>
-  <si>
-    <t>Prov for term3</t>
-  </si>
-  <si>
     <t>ex:XYZ/term3</t>
   </si>
   <si>
-    <t>Prov for term4</t>
-  </si>
-  <si>
     <t>ex:XYZ/term4</t>
   </si>
   <si>
@@ -455,12 +413,6 @@
     <t>AltLbl for term4</t>
   </si>
   <si>
-    <t>ex:test/term5</t>
-  </si>
-  <si>
-    <t>ex:test/term6</t>
-  </si>
-  <si>
     <t>term5</t>
   </si>
   <si>
@@ -470,9 +422,6 @@
     <t>AltLbl for term5</t>
   </si>
   <si>
-    <t>Prov for term5</t>
-  </si>
-  <si>
     <t>ex:XYZ/term5</t>
   </si>
   <si>
@@ -485,18 +434,9 @@
     <t>AltLbl for term6</t>
   </si>
   <si>
-    <t>Prov for term6</t>
-  </si>
-  <si>
     <t>ex:XYZ/term6</t>
   </si>
   <si>
-    <t>ex:test/connected</t>
-  </si>
-  <si>
-    <t>Prov for connected concepts</t>
-  </si>
-  <si>
     <t>def for con</t>
   </si>
   <si>
@@ -504,13 +444,55 @@
   </si>
   <si>
     <t>ex:test/</t>
+  </si>
+  <si>
+    <t>ex:test10</t>
+  </si>
+  <si>
+    <t>ex:test01</t>
+  </si>
+  <si>
+    <t>ex:test02</t>
+  </si>
+  <si>
+    <t>ex:test03</t>
+  </si>
+  <si>
+    <t>ex:test04</t>
+  </si>
+  <si>
+    <t>ex:test05</t>
+  </si>
+  <si>
+    <t>ex:test06</t>
+  </si>
+  <si>
+    <t>ex:test02, ex:test03</t>
+  </si>
+  <si>
+    <t>ex:test01,
+ex:test02,
+ex:test03,
+ex:test04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and distributed under  BSD-3-Clause License </t>
+  </si>
+  <si>
+    <t>0000-0001-2345-6789</t>
+  </si>
+  <si>
+    <t>sofia-garcia</t>
+  </si>
+  <si>
+    <t>Sofia Garcia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -574,13 +556,6 @@
     <font>
       <sz val="10"/>
       <color theme="4" tint="-0.499984740745262"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -662,7 +637,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -712,7 +687,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -730,13 +705,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -745,32 +720,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -782,6 +751,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -791,7 +763,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -799,30 +771,8 @@
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="7">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB47CFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB47CFF"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFD9EAD3"/>
@@ -1109,7 +1059,9 @@
   </sheetPr>
   <dimension ref="A1:K1005"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1134,7 +1086,7 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="34" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="33"/>
@@ -1201,7 +1153,7 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="34" t="s">
         <v>1</v>
       </c>
       <c r="I7" s="33"/>
@@ -1217,7 +1169,7 @@
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
       <c r="H8" s="35" t="s">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="I8" s="33"/>
       <c r="J8" s="33"/>
@@ -1231,7 +1183,7 @@
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="36"/>
+      <c r="H9" s="35"/>
       <c r="I9" s="33"/>
       <c r="J9" s="33"/>
       <c r="K9" s="19"/>
@@ -1244,8 +1196,8 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="36" t="s">
-        <v>3</v>
+      <c r="H10" s="35" t="s">
+        <v>2</v>
       </c>
       <c r="I10" s="33"/>
       <c r="J10" s="33"/>
@@ -1261,10 +1213,10 @@
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
       <c r="I11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="8" t="s">
         <v>4</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>5</v>
       </c>
       <c r="K11" s="19"/>
     </row>
@@ -1289,8 +1241,8 @@
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
-      <c r="H13" s="38" t="s">
-        <v>6</v>
+      <c r="H13" s="36" t="s">
+        <v>5</v>
       </c>
       <c r="I13" s="33"/>
       <c r="J13" s="33"/>
@@ -1304,8 +1256,8 @@
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="36" t="s">
-        <v>7</v>
+      <c r="H14" s="35" t="s">
+        <v>6</v>
       </c>
       <c r="I14" s="33"/>
       <c r="J14" s="33"/>
@@ -1325,12 +1277,12 @@
       <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="C16" s="38" t="s">
         <v>8</v>
-      </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="40" t="s">
-        <v>9</v>
       </c>
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
@@ -1342,12 +1294,12 @@
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="33"/>
+      <c r="C17" s="39" t="s">
         <v>10</v>
-      </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="34" t="s">
-        <v>11</v>
       </c>
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
@@ -1372,8 +1324,8 @@
       <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="37" t="s">
-        <v>12</v>
+      <c r="A19" s="32" t="s">
+        <v>11</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="33"/>
@@ -1426,8 +1378,8 @@
       <c r="K22" s="19"/>
     </row>
     <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="36" t="s">
-        <v>13</v>
+      <c r="A23" s="35" t="s">
+        <v>12</v>
       </c>
       <c r="B23" s="33"/>
       <c r="C23" s="33"/>
@@ -1454,8 +1406,8 @@
       <c r="K24" s="19"/>
     </row>
     <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="37" t="s">
-        <v>14</v>
+      <c r="A25" s="32" t="s">
+        <v>13</v>
       </c>
       <c r="B25" s="33"/>
       <c r="C25" s="33"/>
@@ -1482,8 +1434,8 @@
       <c r="K26" s="19"/>
     </row>
     <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="37" t="s">
-        <v>15</v>
+      <c r="A27" s="32" t="s">
+        <v>14</v>
       </c>
       <c r="B27" s="33"/>
       <c r="C27" s="33"/>
@@ -2488,6 +2440,11 @@
     <row r="1005" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="A25:G25"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="H10:J10"/>
@@ -2498,50 +2455,35 @@
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="A25:G25"/>
   </mergeCells>
-  <conditionalFormatting sqref="H17:J18 K1:K8 K17:K28 H3:J7 H10:J10 H8 K10:K15 H13:J13 H14 A18:G18 A15:J15 A19:J28 A10:G14 A2:G8 A1:J1 A9:K9">
-    <cfRule type="containsBlanks" dxfId="8" priority="13">
+  <conditionalFormatting sqref="A16:C17">
+    <cfRule type="containsBlanks" dxfId="6" priority="3">
+      <formula>LEN(TRIM(A16))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:G2 A3:J4">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="14">
+      <formula>LEN(TRIM(A2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:J1 K1:K8 A2:G8 H8 A9:K9 H10:J10 A10:G14 K10:K15 H14 A15:J15 H17:J18 K17:K28 A18:G18 A19:J28">
+    <cfRule type="containsBlanks" dxfId="4" priority="13">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:J4 A2:G2">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="14">
-      <formula>LEN(TRIM(A2))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17:B17">
-    <cfRule type="containsBlanks" dxfId="6" priority="10">
-      <formula>LEN(TRIM(A17))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:J2">
-    <cfRule type="containsBlanks" dxfId="5" priority="7">
+  <conditionalFormatting sqref="H2:J7">
+    <cfRule type="containsBlanks" dxfId="3" priority="7">
       <formula>LEN(TRIM(H2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16 H16:K16">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(C16))=0</formula>
+  <conditionalFormatting sqref="H12:J13">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
+      <formula>LEN(TRIM(H12))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16:B16">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(A16))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(C17))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H12:J12">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(H12))=0</formula>
+  <conditionalFormatting sqref="H16:K16">
+    <cfRule type="containsBlanks" dxfId="1" priority="5">
+      <formula>LEN(TRIM(H16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -2560,8 +2502,8 @@
   </sheetPr>
   <dimension ref="A1:D999"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2573,8 +2515,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
-        <v>16</v>
+      <c r="A1" s="40" t="s">
+        <v>15</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -2582,154 +2524,154 @@
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="9">
         <v>44896</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="9">
         <v>44896</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="17" t="s">
         <v>32</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>32</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5710,8 +5652,8 @@
   </sheetPr>
   <dimension ref="A1:I523"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5728,211 +5670,211 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
+      <c r="A1" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="2" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="G2" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>54</v>
-      </c>
       <c r="I2" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="G3" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="I3" s="27" t="s">
         <v>79</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="27" t="s">
         <v>88</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>101</v>
       </c>
       <c r="G4" s="24"/>
       <c r="H4" s="27" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="G6" s="28"/>
       <c r="H6" s="27" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="G7" s="28"/>
       <c r="H7" s="27" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6474,7 +6416,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -6489,7 +6431,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6499,60 +6441,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
+      <c r="A1" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="str">
         <f>IFERROR(HLOOKUP(Concepts!A3,Concepts!A3:A523,1), "")</f>
-        <v>ex:test/term1</v>
+        <v>ex:test01</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="str">
         <f>IFERROR(HLOOKUP(Concepts!A4,Concepts!A4:A524,1), "")</f>
-        <v>ex:test/term2</v>
+        <v>ex:test02</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -6563,7 +6505,7 @@
     <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="str">
         <f>IFERROR(HLOOKUP(Concepts!A5,Concepts!A5:A525,1), "")</f>
-        <v>ex:test/term3</v>
+        <v>ex:test03</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -6574,7 +6516,7 @@
     <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="str">
         <f>IFERROR(HLOOKUP(Concepts!A6,Concepts!A6:A526,1), "")</f>
-        <v>ex:test/term4</v>
+        <v>ex:test04</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -6585,7 +6527,7 @@
     <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="str">
         <f>IFERROR(HLOOKUP(Concepts!A7,Concepts!A7:A527,1), "")</f>
-        <v>ex:test/term5</v>
+        <v>ex:test05</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -6596,7 +6538,7 @@
     <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="str">
         <f>IFERROR(HLOOKUP(Concepts!A8,Concepts!A8:A528,1), "")</f>
-        <v>ex:test/term6</v>
+        <v>ex:test06</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -6630,7 +6572,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="A3:A10">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A3))=0</formula>
@@ -6648,7 +6590,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6661,46 +6603,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="A1" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="D2" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>66</v>
-      </c>
       <c r="E2" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>117</v>
+        <v>110</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -6745,18 +6687,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Revised handling of Additional Concept Features sheet.
Update test Excel files to test new handling of Add.Con.Feat. sheet.
Add __init__.py file to tests directory  following pytest best practices.
Reformats imports with ruff 0.9.3
</commit_message>
<xml_diff>
--- a/tests/data/concept-scheme-simple.xlsx
+++ b/tests/data/concept-scheme-simple.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-tool\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\MyProg\gh-nfdi4cat\voc4cat-tool\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C71C26-CD73-41A5-B4F0-10140999E549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA04127F-51E4-4898-A968-79B2E6BC47B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25095" windowHeight="15825" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="115">
   <si>
     <t xml:space="preserve">Created by </t>
   </si>
@@ -732,14 +732,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -749,9 +752,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -771,7 +771,15 @@
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1086,7 +1094,7 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="32" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="33"/>
@@ -1153,7 +1161,7 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="32" t="s">
         <v>1</v>
       </c>
       <c r="I7" s="33"/>
@@ -1241,7 +1249,7 @@
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
-      <c r="H13" s="36" t="s">
+      <c r="H13" s="37" t="s">
         <v>5</v>
       </c>
       <c r="I13" s="33"/>
@@ -1277,11 +1285,11 @@
       <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="38" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="33"/>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="39" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="33"/>
@@ -1294,11 +1302,11 @@
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="38" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="33"/>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="34" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="33"/>
@@ -1324,7 +1332,7 @@
       <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="33"/>
@@ -1406,7 +1414,7 @@
       <c r="K24" s="19"/>
     </row>
     <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="36" t="s">
         <v>13</v>
       </c>
       <c r="B25" s="33"/>
@@ -1434,7 +1442,7 @@
       <c r="K26" s="19"/>
     </row>
     <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="36" t="s">
         <v>14</v>
       </c>
       <c r="B27" s="33"/>
@@ -2440,11 +2448,6 @@
     <row r="1005" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="A25:G25"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="H10:J10"/>
@@ -2455,34 +2458,39 @@
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="A25:G25"/>
   </mergeCells>
   <conditionalFormatting sqref="A16:C17">
-    <cfRule type="containsBlanks" dxfId="6" priority="3">
+    <cfRule type="containsBlanks" dxfId="7" priority="3">
       <formula>LEN(TRIM(A16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:G2 A3:J4">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="14">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:J1 K1:K8 A2:G8 H8 A9:K9 H10:J10 A10:G14 K10:K15 H14 A15:J15 H17:J18 K17:K28 A18:G18 A19:J28">
-    <cfRule type="containsBlanks" dxfId="4" priority="13">
+    <cfRule type="containsBlanks" dxfId="5" priority="13">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J7">
-    <cfRule type="containsBlanks" dxfId="3" priority="7">
+    <cfRule type="containsBlanks" dxfId="4" priority="7">
       <formula>LEN(TRIM(H2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J13">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(H12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:K16">
-    <cfRule type="containsBlanks" dxfId="1" priority="5">
+    <cfRule type="containsBlanks" dxfId="2" priority="5">
       <formula>LEN(TRIM(H16))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2502,7 +2510,7 @@
   </sheetPr>
   <dimension ref="A1:D999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6430,8 +6438,8 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6471,30 +6479,18 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="str">
-        <f>IFERROR(HLOOKUP(Concepts!A3,Concepts!A3:A523,1), "")</f>
-        <v>ex:test01</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="A3" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="str">
-        <f>IFERROR(HLOOKUP(Concepts!A4,Concepts!A4:A524,1), "")</f>
-        <v>ex:test02</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -6503,9 +6499,8 @@
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="str">
-        <f>IFERROR(HLOOKUP(Concepts!A5,Concepts!A5:A525,1), "")</f>
-        <v>ex:test03</v>
+      <c r="A5" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -6514,21 +6509,26 @@
       <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="str">
-        <f>IFERROR(HLOOKUP(Concepts!A6,Concepts!A6:A526,1), "")</f>
-        <v>ex:test04</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="A6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="str">
-        <f>IFERROR(HLOOKUP(Concepts!A7,Concepts!A7:A527,1), "")</f>
-        <v>ex:test05</v>
-      </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -6536,10 +6536,6 @@
       <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="str">
-        <f>IFERROR(HLOOKUP(Concepts!A8,Concepts!A8:A528,1), "")</f>
-        <v>ex:test06</v>
-      </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -6547,10 +6543,6 @@
       <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="str">
-        <f>IFERROR(HLOOKUP(Concepts!A9,Concepts!A9:A529,1), "")</f>
-        <v/>
-      </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -6558,10 +6550,6 @@
       <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="str">
-        <f>IFERROR(HLOOKUP(Concepts!A10,Concepts!A10:A530,1), "")</f>
-        <v/>
-      </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -6573,11 +6561,6 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
-  <conditionalFormatting sqref="A3:A10">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A3))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add test with missing source vocab URI
</commit_message>
<xml_diff>
--- a/tests/data/concept-scheme-simple.xlsx
+++ b/tests/data/concept-scheme-simple.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\MyProg\gh-nfdi4cat\voc4cat-tool\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-tool\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA04127F-51E4-4898-A968-79B2E6BC47B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D9155E-BFBC-4487-8CA6-C976761F58F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="24630" windowHeight="13725" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="114">
   <si>
     <t xml:space="preserve">Created by </t>
   </si>
@@ -432,9 +432,6 @@
   </si>
   <si>
     <t>AltLbl for term6</t>
-  </si>
-  <si>
-    <t>ex:XYZ/term6</t>
   </si>
   <si>
     <t>def for con</t>
@@ -732,17 +729,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -752,6 +746,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -771,23 +768,7 @@
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FFB47CFF"/>
@@ -1094,7 +1075,7 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="34" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="33"/>
@@ -1161,7 +1142,7 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="34" t="s">
         <v>1</v>
       </c>
       <c r="I7" s="33"/>
@@ -1177,7 +1158,7 @@
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
       <c r="H8" s="35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I8" s="33"/>
       <c r="J8" s="33"/>
@@ -1249,7 +1230,7 @@
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
-      <c r="H13" s="37" t="s">
+      <c r="H13" s="36" t="s">
         <v>5</v>
       </c>
       <c r="I13" s="33"/>
@@ -1285,11 +1266,11 @@
       <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="37" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="33"/>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="38" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="33"/>
@@ -1302,11 +1283,11 @@
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="37" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="33"/>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="39" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="33"/>
@@ -1332,7 +1313,7 @@
       <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="33"/>
@@ -1414,7 +1395,7 @@
       <c r="K24" s="19"/>
     </row>
     <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="32" t="s">
         <v>13</v>
       </c>
       <c r="B25" s="33"/>
@@ -1442,7 +1423,7 @@
       <c r="K26" s="19"/>
     </row>
     <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="32" t="s">
         <v>14</v>
       </c>
       <c r="B27" s="33"/>
@@ -2448,6 +2429,11 @@
     <row r="1005" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="A25:G25"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="H10:J10"/>
@@ -2458,39 +2444,34 @@
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="A25:G25"/>
   </mergeCells>
   <conditionalFormatting sqref="A16:C17">
-    <cfRule type="containsBlanks" dxfId="7" priority="3">
+    <cfRule type="containsBlanks" dxfId="5" priority="3">
       <formula>LEN(TRIM(A16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:G2 A3:J4">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="14">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:J1 K1:K8 A2:G8 H8 A9:K9 H10:J10 A10:G14 K10:K15 H14 A15:J15 H17:J18 K17:K28 A18:G18 A19:J28">
-    <cfRule type="containsBlanks" dxfId="5" priority="13">
+    <cfRule type="containsBlanks" dxfId="3" priority="13">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J7">
-    <cfRule type="containsBlanks" dxfId="4" priority="7">
+    <cfRule type="containsBlanks" dxfId="2" priority="7">
       <formula>LEN(TRIM(H2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J13">
-    <cfRule type="containsBlanks" dxfId="3" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(H12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:K16">
-    <cfRule type="containsBlanks" dxfId="2" priority="5">
+    <cfRule type="containsBlanks" dxfId="0" priority="5">
       <formula>LEN(TRIM(H16))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2510,8 +2491,8 @@
   </sheetPr>
   <dimension ref="A1:D999"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2535,7 +2516,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>17</v>
@@ -2647,7 +2628,7 @@
         <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>39</v>
@@ -2661,7 +2642,7 @@
         <v>40</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>41</v>
@@ -5661,7 +5642,7 @@
   <dimension ref="A1:I523"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5721,7 +5702,7 @@
     </row>
     <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>71</v>
@@ -5739,10 +5720,10 @@
         <v>87</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I3" s="27" t="s">
         <v>79</v>
@@ -5750,7 +5731,7 @@
     </row>
     <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>75</v>
@@ -5769,7 +5750,7 @@
       </c>
       <c r="G4" s="24"/>
       <c r="H4" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I4" s="27" t="s">
         <v>80</v>
@@ -5777,7 +5758,7 @@
     </row>
     <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>72</v>
@@ -5795,10 +5776,10 @@
         <v>89</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I5" s="27" t="s">
         <v>81</v>
@@ -5806,7 +5787,7 @@
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" s="26" t="s">
         <v>76</v>
@@ -5825,7 +5806,7 @@
       </c>
       <c r="G6" s="28"/>
       <c r="H6" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I6" s="27" t="s">
         <v>82</v>
@@ -5833,7 +5814,7 @@
     </row>
     <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" s="26" t="s">
         <v>91</v>
@@ -5852,7 +5833,7 @@
       </c>
       <c r="G7" s="28"/>
       <c r="H7" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I7" s="27" t="s">
         <v>94</v>
@@ -5860,7 +5841,7 @@
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>95</v>
@@ -5879,11 +5860,9 @@
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="I8" s="27" t="s">
-        <v>98</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="I8" s="27"/>
     </row>
     <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24"/>
@@ -6438,7 +6417,7 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -6480,7 +6459,7 @@
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -6490,7 +6469,7 @@
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -6500,7 +6479,7 @@
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -6510,22 +6489,22 @@
     </row>
     <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>107</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6613,19 +6592,19 @@
     </row>
     <row r="3" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>